<commit_message>
separated timediff into timediff.xlsx
</commit_message>
<xml_diff>
--- a/DSU_FOP_Data/FOP Course Design_teachers/timestamps.xlsx
+++ b/DSU_FOP_Data/FOP Course Design_teachers/timestamps.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Kavya Alse</t>
   </si>
@@ -22,9 +22,6 @@
     <t>Programming Environment.</t>
   </si>
   <si>
-    <t>0:09:30</t>
-  </si>
-  <si>
     <t>2021-06-07T08:37:43.348Z</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
   </si>
   <si>
     <t>Arjun CSE</t>
-  </si>
-  <si>
-    <t>0:00:00</t>
   </si>
   <si>
     <t>2021-05-07T08:34:36.518Z</t>
@@ -399,13 +393,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,25 +439,19 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" t="s">
-        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>